<commit_message>
chore: Simplifies instructor information.
</commit_message>
<xml_diff>
--- a/tests/Tutor.Infrastructure.Tests/Integration/DataImport/test-excels/enrollment/seed-instructors.xlsx
+++ b/tests/Tutor.Infrastructure.Tests/Integration/DataImport/test-excels/enrollment/seed-instructors.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TUTOR-EDU\TEST-DATA\enrollment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lubur\Documents\Fakultet\!PROJEKTI\2020-2022 Clean CaDET\PLATFORM\tutor\tests\Tutor.Infrastructure.Tests\Integration\DataImport\test-excels\enrollment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AF419EA-7772-4999-9416-2816156F88FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9A8106B-EE0E-4E9B-9245-9FAB6B4D4563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>Name</t>
   </si>
@@ -51,12 +51,6 @@
     <t>Luburić</t>
   </si>
   <si>
-    <t>Tutor!1991</t>
-  </si>
-  <si>
-    <t>Tutor!1999</t>
-  </si>
-  <si>
     <t>Nataša</t>
   </si>
   <si>
@@ -72,9 +66,6 @@
     <t>simona.prokic</t>
   </si>
   <si>
-    <t>Tutor!1998</t>
-  </si>
-  <si>
     <t>Luka</t>
   </si>
   <si>
@@ -84,7 +75,7 @@
     <t>luka.doric</t>
   </si>
   <si>
-    <t>Tutor!1995</t>
+    <t>tutor</t>
   </si>
 </sst>
 </file>
@@ -432,7 +423,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -465,49 +456,49 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
         <v>16</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>